<commit_message>
first runnable core build
</commit_message>
<xml_diff>
--- a/textclassifier2_core/test_db/test.xlsx
+++ b/textclassifier2_core/test_db/test.xlsx
@@ -21,12 +21,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Characteristic 1</t>
-  </si>
-  <si>
-    <t>Characteristic 2</t>
-  </si>
-  <si>
     <t>Требуется починить телефон</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>Методисты</t>
+  </si>
+  <si>
+    <t>Отдел</t>
+  </si>
+  <si>
+    <t>Тип</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,76 +427,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>